<commit_message>
commit new version of bom, cpl, and rar file for REV D of SGMS
</commit_message>
<xml_diff>
--- a/Diptrace/Gerber/SGMS REVD Support Files/SGMS RevD BOM.xlsx
+++ b/Diptrace/Gerber/SGMS REVD Support Files/SGMS RevD BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brenn\Desktop\Baja\Github\not-code\Diptrace\Gerber\SGMS REVD Support Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C914C43-BDE2-42A8-ADA9-C88EBDC9EAAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F9545B-9DEF-4B8B-BB08-C0D59581EC94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="1760" windowWidth="9180" windowHeight="9590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,10 +72,10 @@
     <t>TS972IDT</t>
   </si>
   <si>
-    <t>SOIC-8_150mil</t>
-  </si>
-  <si>
     <t>C183638</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -483,10 +483,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" customHeight="1"/>

</xml_diff>